<commit_message>
feat(gerar_relatorio): Implementada a geração do csv e xlsx.
</commit_message>
<xml_diff>
--- a/vendas.xlsx
+++ b/vendas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,25 +463,160 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>cli-9876</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ana schmidt</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10/10/2025</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>r$ 250,75</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['- item a: 1 unidade', '- item b: 3 unidades']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>cli-9876</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ana schmidt</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10/10/2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>r$ 250,75</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['- item a: 1 unidade', '- item b: 3 unidades']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>cli-5432</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>bruno costa</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>12/10/2025</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>r$ 1.120,00</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['- item c: 10 unidades', '- item d: 1 unidade']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>cli-9876</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ana schmidt</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10/10/2025</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>r$ 250,75</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['- item a: 1 unidade', '- item b: 3 unidades']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>cli-9876</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ana schmidt</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10/10/2025</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>r$ 250,75</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['- item a: 1 unidade', '- item b: 3 unidades']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>cli-5432</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>bruno costa</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12/10/2025</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>r$ 1.120,00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>['- item c: 10 unidades', '- item d: 1 unidade']</t>
         </is>

</xml_diff>